<commit_message>
moved main graph to first sheet #37
</commit_message>
<xml_diff>
--- a/Data/Finding Time Till Block/timeTillBlockData.xlsx
+++ b/Data/Finding Time Till Block/timeTillBlockData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\Stuff\Code\Nerve-Block-Modeling\Data\Finding Time Till Block\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D203F377-9163-4522-B242-EEFBEFEAAA95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70E2343-FBA5-49B0-9408-1AC315561219}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{8172BA03-0129-43C9-BC80-8657147BC1FE}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="25416" windowHeight="15372" xr2:uid="{8172BA03-0129-43C9-BC80-8657147BC1FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="10um diam" sheetId="1" r:id="rId1"/>
-    <sheet name="12.8um diam" sheetId="2" r:id="rId2"/>
-    <sheet name="7.3um diam" sheetId="3" r:id="rId3"/>
+    <sheet name="Chart1" sheetId="4" r:id="rId1"/>
+    <sheet name="10um diam" sheetId="1" r:id="rId2"/>
+    <sheet name="12.8um diam" sheetId="2" r:id="rId3"/>
+    <sheet name="7.3um diam" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,6 +115,649 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t>Wait Time After Last AP Passes Node[30]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>600000nA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'10um diam'!$B$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'10um diam'!$B$15:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.1007809999999978</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1437499999999972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1781249999999979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2210939999999972</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2554689999999979</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2898439999999987</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3242189999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3585940000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3843749999999986</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4101560000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4359369999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-877C-47C2-8CF6-D5BA0C4BF94D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>700000nA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'10um diam'!$B$21:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'10um diam'!$B$34:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.80859399999999937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80859399999999937</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83437499999999964</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89453099999999885</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95468700000000162</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98906199999999878</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0320310000000017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0750000000000011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1007809999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1351560000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.169531000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-877C-47C2-8CF6-D5BA0C4BF94D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="601574968"/>
+        <c:axId val="601573048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="601574968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>Node</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601573048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="601573048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t>Wait Time After Last AP (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="601574968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1189,7 +1833,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2016,7 +2660,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2671,654 +3315,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" baseline="0"/>
-              <a:t>Wait Time After Last AP Passes Node[30]</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>600000nA</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'10um diam'!$B$2:$L$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'10um diam'!$B$15:$L$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1.1007809999999978</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1437499999999972</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.1781249999999979</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2210939999999972</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2554689999999979</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2898439999999987</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3242189999999994</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.3585940000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.3843749999999986</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.4101560000000006</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.4359369999999991</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A7A7-4B98-B5FE-043D06BF7A14}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>700000nA</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'10um diam'!$B$21:$L$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>40</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'10um diam'!$B$34:$L$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.80859399999999937</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.80859399999999937</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.83437499999999964</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.89453099999999885</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.95468700000000162</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.98906199999999878</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0320310000000017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0750000000000011</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1007809999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.1351560000000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.169531000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A7A7-4B98-B5FE-043D06BF7A14}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="601574968"/>
-        <c:axId val="601573048"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="601574968"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="30"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                  <a:t>Node</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="601573048"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="601573048"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0.70000000000000007"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                  <a:t>Wait Time After Last AP (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1600"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="601574968"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -6667,7 +6663,51 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{46D468C1-40FB-40A5-AA60-AAF5A8F98448}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656053" cy="6283158"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114C6FB7-560B-4E06-B909-D630C2ECC108}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6777,59 +6817,23 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>480059</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>169544</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC684F12-8266-4021-A319-99E593CD193C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>48577</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>170497</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>75247</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7156,7 +7160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EF7CF3-170A-465C-BD80-C479764B0D9D}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
@@ -8779,7 +8783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0534871-47CF-44A4-9697-367506944F87}">
   <dimension ref="A2:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>